<commit_message>
[RF] debuggging Data update
</commit_message>
<xml_diff>
--- a/1_Schematic/Build V2.0/RF-GEN-Test Date_20200207.xlsx
+++ b/1_Schematic/Build V2.0/RF-GEN-Test Date_20200207.xlsx
@@ -1,22 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22430"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A6C88DD-45AA-4F53-B8BB-3FA1AA64D3A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SET" sheetId="1" r:id="rId1"/>
     <sheet name="RF" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="48">
   <si>
     <t>12V</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -99,17 +108,126 @@
   </si>
   <si>
     <t>Calcul</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SIG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gain이 안올라감</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>meas</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tune2/8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R24 NC 상태에서도 동일함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PWR tune후 연결하여 Test할때 R24 NC 처리 여부 결정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PWR LT1210CT7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CPU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C8/C11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100nF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C9/C10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100pF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10K</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IOUTB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gain</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RFIN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>무부하</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>종단</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Iout</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
     <numFmt numFmtId="176" formatCode="&quot;#&quot;00"/>
+    <numFmt numFmtId="180" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,8 +251,29 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -147,8 +286,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -310,7 +461,7 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
@@ -322,6 +473,32 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -331,16 +508,27 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -354,21 +542,85 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="180" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="180" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="180" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="180" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="180" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="180" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -378,6 +630,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -426,7 +681,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -459,9 +714,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -494,6 +766,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -669,21 +958,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <sheetData>
-    <row r="2" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:8" ht="18" thickBot="1">
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8">
       <c r="B3" s="4"/>
       <c r="C3" s="5">
         <v>1</v>
@@ -704,7 +993,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8">
       <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
@@ -727,7 +1016,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8">
       <c r="B5" s="7" t="s">
         <v>0</v>
       </c>
@@ -750,7 +1039,7 @@
         <v>11.98</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8">
       <c r="B6" s="7" t="s">
         <v>5</v>
       </c>
@@ -779,7 +1068,7 @@
         <v>0.83860000000000012</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:8">
       <c r="B7" s="7" t="s">
         <v>2</v>
       </c>
@@ -802,7 +1091,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8">
       <c r="B8" s="7" t="s">
         <v>3</v>
       </c>
@@ -825,7 +1114,7 @@
         <v>3.3050000000000002</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8">
       <c r="B9" s="7" t="s">
         <v>6</v>
       </c>
@@ -848,7 +1137,7 @@
         <v>3.3029999999999999</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:8" ht="18" thickBot="1">
       <c r="B10" s="10" t="s">
         <v>7</v>
       </c>
@@ -878,118 +1167,894 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:L7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="B3:Q31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="1" max="2" width="6.625" customWidth="1"/>
-    <col min="3" max="3" width="9.25" customWidth="1"/>
-    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.625" customWidth="1"/>
+    <col min="1" max="2" width="6.59765625" customWidth="1"/>
+    <col min="3" max="4" width="9.19921875" customWidth="1"/>
+    <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:17" ht="18" thickBot="1">
       <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C5" s="14"/>
-      <c r="D5" s="15" t="s">
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="2:17" s="18" customFormat="1">
+      <c r="C4" s="46"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="M4" s="26"/>
+      <c r="N4" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="O4" s="26"/>
+      <c r="P4" s="48"/>
+    </row>
+    <row r="5" spans="2:17" s="18" customFormat="1" ht="18" thickBot="1">
+      <c r="C5" s="49"/>
+      <c r="D5" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="F5" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="G5" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="H5" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" s="15" t="s">
+      <c r="I5" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="J5" s="15" t="s">
+      <c r="J5" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="K5" s="15" t="s">
+      <c r="K5" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="L5" s="17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C6" s="20" t="s">
+      <c r="L5" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="M5" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="N5" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="O5" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="P5" s="29" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17">
+      <c r="C6" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="36"/>
+      <c r="E6" s="37">
         <v>0.6</v>
       </c>
-      <c r="E6" s="13">
+      <c r="F6" s="17">
         <v>470</v>
       </c>
-      <c r="F6" s="13">
+      <c r="G6" s="17">
         <v>47</v>
       </c>
-      <c r="G6" s="13">
-        <f>1+E6/F6</f>
+      <c r="H6" s="37">
+        <f>1+F6/G6</f>
         <v>11</v>
       </c>
-      <c r="H6" s="18">
-        <f>D6*G6</f>
+      <c r="I6" s="17">
+        <v>51</v>
+      </c>
+      <c r="J6" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="K6" s="17">
+        <v>51</v>
+      </c>
+      <c r="L6" s="16">
+        <f>E6*H6</f>
         <v>6.6</v>
       </c>
-      <c r="I6" s="13">
+      <c r="M6" s="13"/>
+      <c r="N6" s="16">
+        <f>L6*K6/(I6+K6)</f>
+        <v>3.3</v>
+      </c>
+      <c r="O6" s="13"/>
+      <c r="P6" s="30">
+        <f>N6*N6/K6</f>
+        <v>0.21352941176470586</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17">
+      <c r="C7" s="31"/>
+      <c r="D7" s="38">
+        <v>0.6</v>
+      </c>
+      <c r="E7" s="39">
+        <v>0.4</v>
+      </c>
+      <c r="F7" s="21">
+        <v>470</v>
+      </c>
+      <c r="G7" s="21">
+        <v>47</v>
+      </c>
+      <c r="H7" s="39">
+        <f>1+F7/G7</f>
+        <v>11</v>
+      </c>
+      <c r="I7" s="21">
         <v>51</v>
       </c>
-      <c r="J6" s="13" t="s">
+      <c r="J7" s="21">
+        <v>51</v>
+      </c>
+      <c r="K7" s="21">
+        <v>51</v>
+      </c>
+      <c r="L7" s="22">
+        <f>E7*H7</f>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="M7" s="2"/>
+      <c r="N7" s="22">
+        <v>0.7</v>
+      </c>
+      <c r="O7" s="2"/>
+      <c r="P7" s="9">
+        <f>N7*N7/K7</f>
+        <v>9.6078431372549015E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17">
+      <c r="C8" s="7"/>
+      <c r="D8" s="38">
+        <v>0.6</v>
+      </c>
+      <c r="E8" s="39">
+        <v>0.4</v>
+      </c>
+      <c r="F8" s="21">
+        <v>470</v>
+      </c>
+      <c r="G8" s="21">
+        <v>47</v>
+      </c>
+      <c r="H8" s="39">
+        <f>1+F8/G8</f>
+        <v>11</v>
+      </c>
+      <c r="I8" s="21">
+        <v>51</v>
+      </c>
+      <c r="J8" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="K6" s="13">
+      <c r="K8" s="21">
         <v>51</v>
       </c>
-      <c r="L6" s="19">
-        <f>H6*K6/(I6+K6)</f>
+      <c r="L8" s="22">
+        <f>E8*H8</f>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="M8" s="2">
+        <v>2.1</v>
+      </c>
+      <c r="N8" s="22">
+        <f>M8*K8/(I8+K8)</f>
+        <v>1.05</v>
+      </c>
+      <c r="O8" s="2">
+        <v>0.88</v>
+      </c>
+      <c r="P8" s="9">
+        <f>N8*N8/K8</f>
+        <v>2.161764705882353E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17">
+      <c r="C9" s="31"/>
+      <c r="D9" s="38">
+        <v>0.9</v>
+      </c>
+      <c r="E9" s="39">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="F9" s="21">
+        <v>470</v>
+      </c>
+      <c r="G9" s="21">
+        <v>47</v>
+      </c>
+      <c r="H9" s="39">
+        <f>1+F9/G9</f>
+        <v>11</v>
+      </c>
+      <c r="I9" s="21">
+        <v>51</v>
+      </c>
+      <c r="J9" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="K9" s="21">
+        <v>51</v>
+      </c>
+      <c r="L9" s="24">
+        <f>E9*H9</f>
+        <v>6.38</v>
+      </c>
+      <c r="M9" s="2">
+        <v>2.9</v>
+      </c>
+      <c r="N9" s="22">
+        <f>M9*K9/(I9+K9)</f>
+        <v>1.45</v>
+      </c>
+      <c r="O9" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="P9" s="9">
+        <f>O9*O9/K9</f>
+        <v>2.8235294117647056E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17">
+      <c r="C10" s="31"/>
+      <c r="D10" s="38">
+        <v>0.9</v>
+      </c>
+      <c r="E10" s="39">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="F10" s="21">
+        <v>1000</v>
+      </c>
+      <c r="G10" s="21">
+        <v>47</v>
+      </c>
+      <c r="H10" s="40">
+        <f>1+F10/G10</f>
+        <v>22.276595744680851</v>
+      </c>
+      <c r="I10" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" s="21"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="24">
+        <f>E10*H10</f>
+        <v>12.920425531914892</v>
+      </c>
+      <c r="M10" s="2">
+        <v>2.8</v>
+      </c>
+      <c r="N10" s="22"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="8"/>
+    </row>
+    <row r="11" spans="2:17">
+      <c r="C11" s="7"/>
+      <c r="D11" s="38">
+        <v>0.9</v>
+      </c>
+      <c r="E11" s="39">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="F11" s="25">
+        <v>200</v>
+      </c>
+      <c r="G11" s="25">
+        <v>47</v>
+      </c>
+      <c r="H11" s="41">
+        <f>1+F11/G11</f>
+        <v>5.2553191489361701</v>
+      </c>
+      <c r="I11" s="21">
+        <v>51</v>
+      </c>
+      <c r="J11" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="K11" s="21">
+        <v>51</v>
+      </c>
+      <c r="L11" s="24">
+        <f>E11*H11</f>
+        <v>3.0480851063829784</v>
+      </c>
+      <c r="M11" s="21">
+        <v>2.4</v>
+      </c>
+      <c r="N11" s="22">
+        <f>M11*K11/(I11+K11)</f>
+        <v>1.2</v>
+      </c>
+      <c r="O11" s="2">
+        <v>1.04</v>
+      </c>
+      <c r="P11" s="9">
+        <f>O11*O11/K11</f>
+        <v>2.1207843137254906E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17">
+      <c r="C12" s="7"/>
+      <c r="D12" s="38">
+        <v>0.9</v>
+      </c>
+      <c r="E12" s="39">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="F12" s="25">
+        <v>200</v>
+      </c>
+      <c r="G12" s="25">
+        <v>47</v>
+      </c>
+      <c r="H12" s="41">
+        <f>1+F12/G12</f>
+        <v>5.2553191489361701</v>
+      </c>
+      <c r="I12" s="21">
+        <v>51</v>
+      </c>
+      <c r="J12" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="K12" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="L12" s="24">
+        <f>E12*H12</f>
+        <v>3.0480851063829784</v>
+      </c>
+      <c r="M12" s="21">
+        <v>2.64</v>
+      </c>
+      <c r="N12" s="22"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="8"/>
+    </row>
+    <row r="13" spans="2:17">
+      <c r="C13" s="7"/>
+      <c r="D13" s="38">
+        <v>0.9</v>
+      </c>
+      <c r="E13" s="39">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="F13" s="25">
+        <v>200</v>
+      </c>
+      <c r="G13" s="25">
+        <v>47</v>
+      </c>
+      <c r="H13" s="41">
+        <f>1+F13/G13</f>
+        <v>5.2553191489361701</v>
+      </c>
+      <c r="I13" s="21">
+        <v>0</v>
+      </c>
+      <c r="J13" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="K13" s="21">
+        <v>51</v>
+      </c>
+      <c r="L13" s="24">
+        <f>E13*H13</f>
+        <v>3.0480851063829784</v>
+      </c>
+      <c r="M13" s="21">
+        <v>2.8</v>
+      </c>
+      <c r="N13" s="22">
+        <f>M13*K13/(I13+K13)</f>
+        <v>2.8</v>
+      </c>
+      <c r="O13" s="2">
+        <v>3</v>
+      </c>
+      <c r="P13" s="9">
+        <f>O13*O13/K13</f>
+        <v>0.17647058823529413</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17">
+      <c r="C14" s="7"/>
+      <c r="D14" s="38">
+        <v>0.9</v>
+      </c>
+      <c r="E14" s="39">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="F14" s="21">
+        <v>270</v>
+      </c>
+      <c r="G14" s="25">
+        <v>47</v>
+      </c>
+      <c r="H14" s="41">
+        <f>1+F14/G14</f>
+        <v>6.7446808510638299</v>
+      </c>
+      <c r="I14" s="21">
+        <v>0</v>
+      </c>
+      <c r="J14" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="K14" s="21">
+        <v>51</v>
+      </c>
+      <c r="L14" s="24">
+        <f>E14*H14</f>
+        <v>3.9119148936170212</v>
+      </c>
+      <c r="M14" s="21">
+        <v>3.04</v>
+      </c>
+      <c r="N14" s="22">
+        <f>M14*K14/(I14+K14)</f>
+        <v>3.04</v>
+      </c>
+      <c r="O14" s="2">
+        <v>3.32</v>
+      </c>
+      <c r="P14" s="9">
+        <f>O14*O14/K14</f>
+        <v>0.21612549019607841</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17">
+      <c r="C15" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="23">
+        <v>0.9</v>
+      </c>
+      <c r="E15" s="22">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="F15" s="22">
+        <v>470</v>
+      </c>
+      <c r="G15" s="33">
+        <v>47</v>
+      </c>
+      <c r="H15" s="34">
+        <f>1+F15/G15</f>
+        <v>11</v>
+      </c>
+      <c r="I15" s="22">
+        <v>0</v>
+      </c>
+      <c r="J15" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="K15" s="22">
+        <v>51</v>
+      </c>
+      <c r="L15" s="24">
+        <f>E15*H15</f>
+        <v>6.38</v>
+      </c>
+      <c r="M15" s="22">
         <v>3.3</v>
       </c>
-    </row>
-    <row r="7" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="21"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="12"/>
+      <c r="N15" s="22">
+        <f>M15*K15/(I15+K15)</f>
+        <v>3.3</v>
+      </c>
+      <c r="O15" s="22">
+        <v>3.6</v>
+      </c>
+      <c r="P15" s="35">
+        <f>O15*O15/K15</f>
+        <v>0.25411764705882356</v>
+      </c>
+    </row>
+    <row r="16" spans="2:17">
+      <c r="C16" s="7"/>
+      <c r="D16" s="42">
+        <v>0.9</v>
+      </c>
+      <c r="E16" s="43">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="F16" s="43">
+        <v>470</v>
+      </c>
+      <c r="G16" s="43">
+        <v>47</v>
+      </c>
+      <c r="H16" s="44">
+        <f>1+F16/G16</f>
+        <v>11</v>
+      </c>
+      <c r="I16" s="43">
+        <v>0</v>
+      </c>
+      <c r="J16" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="K16" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="L16" s="44">
+        <f>E16*H16</f>
+        <v>6.38</v>
+      </c>
+      <c r="M16" s="43">
+        <v>3.32</v>
+      </c>
+      <c r="N16" s="43"/>
+      <c r="O16" s="43">
+        <v>3.64</v>
+      </c>
+      <c r="P16" s="45"/>
+      <c r="Q16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="2:17" ht="18" thickBot="1">
+      <c r="C17" s="10"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="11"/>
+      <c r="O17" s="11"/>
+      <c r="P17" s="12"/>
+    </row>
+    <row r="18" spans="2:17">
+      <c r="C18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="2:17" ht="18" thickBot="1">
+      <c r="B20" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="2:17" ht="18" thickBot="1">
+      <c r="N21" s="56" t="s">
+        <v>43</v>
+      </c>
+      <c r="O21" s="57"/>
+    </row>
+    <row r="22" spans="2:17" s="50" customFormat="1" ht="18" thickBot="1">
+      <c r="C22" s="51" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="F22" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="G22" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="H22" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="I22" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="J22" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="K22" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="L22" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="M22" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="N22" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="O22" s="52" t="s">
+        <v>24</v>
+      </c>
+      <c r="P22" s="55" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q22" s="50" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="2:17">
+      <c r="C23" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" s="13">
+        <v>51</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="H23" s="13">
+        <v>680</v>
+      </c>
+      <c r="I23" s="13">
+        <v>680</v>
+      </c>
+      <c r="J23" s="54">
+        <f>1+H23/I23</f>
+        <v>2</v>
+      </c>
+      <c r="K23" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="L23" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="M23" s="13">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="N23" s="13">
+        <f>M23*J23</f>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="O23" s="13">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="P23" s="14"/>
+    </row>
+    <row r="24" spans="2:17">
+      <c r="C24" s="7"/>
+      <c r="D24" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H24" s="2">
+        <v>680</v>
+      </c>
+      <c r="I24" s="2">
+        <v>680</v>
+      </c>
+      <c r="J24" s="41">
+        <f>1+H24/I24</f>
+        <v>2</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M24" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="N24" s="2">
+        <f>M24*J24</f>
+        <v>6.6</v>
+      </c>
+      <c r="O24" s="2">
+        <v>7.4</v>
+      </c>
+      <c r="P24" s="8"/>
+    </row>
+    <row r="25" spans="2:17">
+      <c r="C25" s="7"/>
+      <c r="D25" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H25" s="2">
+        <v>680</v>
+      </c>
+      <c r="I25" s="2">
+        <v>680</v>
+      </c>
+      <c r="J25" s="41">
+        <f>1+H25/I25</f>
+        <v>2</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L25" s="2">
+        <v>51</v>
+      </c>
+      <c r="M25" s="2">
+        <v>3.36</v>
+      </c>
+      <c r="N25" s="2">
+        <f>M25*J25</f>
+        <v>6.72</v>
+      </c>
+      <c r="O25" s="2">
+        <v>7.68</v>
+      </c>
+      <c r="P25" s="9">
+        <f>O25*O25/L25</f>
+        <v>1.1565176470588234</v>
+      </c>
+      <c r="Q25">
+        <f>P25/O25</f>
+        <v>0.15058823529411763</v>
+      </c>
+    </row>
+    <row r="26" spans="2:17">
+      <c r="C26" s="7"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="8"/>
+    </row>
+    <row r="27" spans="2:17">
+      <c r="C27" s="7"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="8"/>
+    </row>
+    <row r="28" spans="2:17">
+      <c r="C28" s="7"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+      <c r="P28" s="8"/>
+    </row>
+    <row r="29" spans="2:17">
+      <c r="C29" s="7"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+      <c r="P29" s="8"/>
+    </row>
+    <row r="30" spans="2:17">
+      <c r="C30" s="7"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="8"/>
+    </row>
+    <row r="31" spans="2:17" ht="18" thickBot="1">
+      <c r="C31" s="10"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="11"/>
+      <c r="M31" s="11"/>
+      <c r="N31" s="11"/>
+      <c r="O31" s="11"/>
+      <c r="P31" s="12"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N21:O21"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[RF-GEN]Coupler review data update
</commit_message>
<xml_diff>
--- a/1_Schematic/Build V2.0/RF-GEN-Test Date_20200207.xlsx
+++ b/1_Schematic/Build V2.0/RF-GEN-Test Date_20200207.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22430"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5188336B-C1FF-4A0A-B983-37A601B79990}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="8"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RF" sheetId="2" r:id="rId1"/>
@@ -16,8 +17,9 @@
     <sheet name="FAN" sheetId="4" r:id="rId7"/>
     <sheet name="Sheet1" sheetId="8" r:id="rId8"/>
     <sheet name="Test sheet (2)" sheetId="10" r:id="rId9"/>
+    <sheet name="Coupler" sheetId="11" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="206">
   <si>
     <t>CPU AD8051</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -693,15 +695,236 @@
     <t>NC</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>turn ratio 1:25의 동일한 Transformer 2ea 사용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Irms[A]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Long-wave SWR meter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Circuit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>coupling 1:25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FT114-43</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FT50-43</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Core OD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>uH for 25T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>uH</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Start frequency</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MHz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2차측 impedance</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ω</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2차측 권선 길이</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>m</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>100</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>Ω</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 2W 두개를 사용하여 50Ω 4W 설계</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1) Transformer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2차측 impedance가 Load impedance의 10배의 impedance를 가져야 한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ipp[A]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RF-INPUT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UNIT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2차측 권선의 길이가 가장 짧은 파장의 1/10 이하 이어야 한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>End frequency</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>파장</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2차측 권선 최대 길이</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KΩ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2) rectified circuit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1차</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2차</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R1[KΩ]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R2[KΩ]</t>
+  </si>
+  <si>
+    <t>R2[KΩ]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VT Turn ratio</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CT Turn ratio</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VT - 1차측의 전류는 Load Z와 Trans Z로 계산해야 함.(Transformer 공식 사용하면 안됨)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CT  - 1차측의 전압은 Load Z와 Trans Z로 계산해야 함.(Transformer 공식 사용하면 안됨)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RC Filter 설계</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KHz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>τ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>usec</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bypass Cap</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Z</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
     <numFmt numFmtId="176" formatCode="0.0"/>
+    <numFmt numFmtId="179" formatCode="0.000"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -761,6 +984,19 @@
       <family val="3"/>
       <charset val="129"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -800,7 +1036,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="40">
+  <borders count="48">
     <border>
       <left/>
       <right/>
@@ -1339,11 +1575,115 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="165">
+  <cellXfs count="269">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1580,6 +1920,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1654,6 +2003,193 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="6" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1670,6 +2206,316 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>167640</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>171226</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>132677</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="그림 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC6F77A9-FEA9-45DA-87D2-086B17683761}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5082540" y="5067300"/>
+          <a:ext cx="1344706" cy="643217"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>388620</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>213360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>354817</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>84717</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="그림 2" descr="SWR 브리지의 회로도">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81C3430D-C091-4C50-9B59-A1931072C053}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7985760" y="213360"/>
+          <a:ext cx="6001237" cy="5449197"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>365760</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>205740</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="그림 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3BCAF82E-D8D6-45E0-8C46-F0F1020E5DFB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11315700" y="11094720"/>
+          <a:ext cx="1851660" cy="1889760"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>184938</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="그림 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15DCCD1A-57BD-4EFE-8971-DB6743437742}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5219700" y="11871960"/>
+          <a:ext cx="4732020" cy="1480338"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>449580</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>67705</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="그림 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B13674B6-96A0-4841-A4CF-5F1D17BB2FB0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10294620" y="11879580"/>
+          <a:ext cx="1775460" cy="677305"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1715,7 +2561,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1748,9 +2594,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1783,6 +2646,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1958,22 +2838,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:X31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="1" max="2" width="6.625" customWidth="1"/>
-    <col min="3" max="4" width="9.25" customWidth="1"/>
+    <col min="1" max="2" width="6.59765625" customWidth="1"/>
+    <col min="3" max="4" width="9.19921875" customWidth="1"/>
     <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.625" customWidth="1"/>
+    <col min="6" max="6" width="6.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:24" ht="17.25" thickBot="1">
+    <row r="3" spans="2:24" ht="18" thickBot="1">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1990,17 +2870,17 @@
       <c r="I4" s="43"/>
       <c r="J4" s="43"/>
       <c r="K4" s="43"/>
-      <c r="L4" s="140" t="s">
+      <c r="L4" s="143" t="s">
         <v>4</v>
       </c>
-      <c r="M4" s="140"/>
-      <c r="N4" s="140" t="s">
+      <c r="M4" s="143"/>
+      <c r="N4" s="143" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="140"/>
+      <c r="O4" s="143"/>
       <c r="P4" s="44"/>
     </row>
-    <row r="5" spans="2:24" s="15" customFormat="1" ht="17.25" thickBot="1">
+    <row r="5" spans="2:24" s="15" customFormat="1" ht="18" thickBot="1">
       <c r="C5" s="45"/>
       <c r="D5" s="24" t="s">
         <v>12</v>
@@ -2542,7 +3422,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="2:17" ht="17.25" thickBot="1">
+    <row r="17" spans="2:17" ht="18" thickBot="1">
       <c r="C17" s="7"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
@@ -2563,18 +3443,18 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="2:17" ht="17.25" thickBot="1">
+    <row r="20" spans="2:17" ht="18" thickBot="1">
       <c r="B20" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="2:17" ht="17.25" thickBot="1">
-      <c r="N21" s="141" t="s">
+    <row r="21" spans="2:17" ht="18" thickBot="1">
+      <c r="N21" s="144" t="s">
         <v>34</v>
       </c>
-      <c r="O21" s="142"/>
-    </row>
-    <row r="22" spans="2:17" s="46" customFormat="1" ht="17.25" thickBot="1">
+      <c r="O21" s="145"/>
+    </row>
+    <row r="22" spans="2:17" s="46" customFormat="1" ht="18" thickBot="1">
       <c r="C22" s="47" t="s">
         <v>21</v>
       </c>
@@ -2836,7 +3716,7 @@
       <c r="O30" s="2"/>
       <c r="P30" s="5"/>
     </row>
-    <row r="31" spans="2:17" ht="17.25" thickBot="1">
+    <row r="31" spans="2:17" ht="18" thickBot="1">
       <c r="C31" s="7"/>
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
@@ -2863,18 +3743,1844 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34E61BE2-D52E-4F1A-A460-6E9EC3FBF46E}">
+  <dimension ref="B1:R62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="T44" sqref="T44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
+  <cols>
+    <col min="1" max="3" width="3.8984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:13">
+      <c r="B1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="2:13">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13">
+      <c r="C3" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13">
+      <c r="C4" s="1"/>
+      <c r="D4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" ht="18" thickBot="1">
+      <c r="C5" s="1"/>
+      <c r="D5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13">
+      <c r="C6" s="1"/>
+      <c r="D6" s="190" t="s">
+        <v>177</v>
+      </c>
+      <c r="E6" s="191"/>
+      <c r="F6" s="191"/>
+      <c r="G6" s="191"/>
+      <c r="H6" s="192"/>
+      <c r="I6" s="190" t="s">
+        <v>160</v>
+      </c>
+      <c r="J6" s="191"/>
+      <c r="K6" s="191"/>
+      <c r="L6" s="191"/>
+      <c r="M6" s="192"/>
+    </row>
+    <row r="7" spans="2:13" ht="18" thickBot="1">
+      <c r="C7" s="1"/>
+      <c r="D7" s="193" t="s">
+        <v>115</v>
+      </c>
+      <c r="E7" s="194" t="s">
+        <v>114</v>
+      </c>
+      <c r="F7" s="194" t="s">
+        <v>113</v>
+      </c>
+      <c r="G7" s="194" t="s">
+        <v>157</v>
+      </c>
+      <c r="H7" s="195" t="s">
+        <v>176</v>
+      </c>
+      <c r="I7" s="200" t="s">
+        <v>114</v>
+      </c>
+      <c r="J7" s="201" t="s">
+        <v>113</v>
+      </c>
+      <c r="K7" s="201" t="s">
+        <v>115</v>
+      </c>
+      <c r="L7" s="201" t="s">
+        <v>157</v>
+      </c>
+      <c r="M7" s="202" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13">
+      <c r="C8" s="1"/>
+      <c r="D8" s="3">
+        <v>10</v>
+      </c>
+      <c r="E8" s="169">
+        <f>(D8*50)^0.5</f>
+        <v>22.360679774997898</v>
+      </c>
+      <c r="F8" s="169">
+        <f>E8/0.707*2</f>
+        <v>63.255105445538611</v>
+      </c>
+      <c r="G8" s="169">
+        <f>D8/E8</f>
+        <v>0.44721359549995793</v>
+      </c>
+      <c r="H8" s="185">
+        <f>G8/0.707*2</f>
+        <v>1.2651021089107721</v>
+      </c>
+      <c r="I8" s="170">
+        <f>E8/25</f>
+        <v>0.89442719099991597</v>
+      </c>
+      <c r="J8" s="169">
+        <f>I8/0.707*2</f>
+        <v>2.5302042178215447</v>
+      </c>
+      <c r="K8" s="56">
+        <f>I8*I8/50</f>
+        <v>1.6000000000000004E-2</v>
+      </c>
+      <c r="L8" s="56">
+        <f>K8/I8</f>
+        <v>1.7888543819998319E-2</v>
+      </c>
+      <c r="M8" s="185">
+        <f>L8/0.707*2</f>
+        <v>5.0604084356430892E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13">
+      <c r="C9" s="1"/>
+      <c r="D9" s="4">
+        <v>100</v>
+      </c>
+      <c r="E9" s="103">
+        <f t="shared" ref="E9:E12" si="0">(D9*50)^0.5</f>
+        <v>70.710678118654755</v>
+      </c>
+      <c r="F9" s="103">
+        <f>E9/0.707*2</f>
+        <v>200.03020684202195</v>
+      </c>
+      <c r="G9" s="103">
+        <f t="shared" ref="G9:G12" si="1">D9/E9</f>
+        <v>1.4142135623730949</v>
+      </c>
+      <c r="H9" s="108">
+        <f t="shared" ref="H9:H12" si="2">G9/0.707*2</f>
+        <v>4.0006041368404386</v>
+      </c>
+      <c r="I9" s="171">
+        <f>E9/25</f>
+        <v>2.8284271247461903</v>
+      </c>
+      <c r="J9" s="103">
+        <f t="shared" ref="J9:J12" si="3">I9/0.707*2</f>
+        <v>8.0012082736808789</v>
+      </c>
+      <c r="K9" s="172">
+        <f t="shared" ref="K9:K12" si="4">I9*I9/50</f>
+        <v>0.16000000000000003</v>
+      </c>
+      <c r="L9" s="172">
+        <f t="shared" ref="L9:L12" si="5">K9/I9</f>
+        <v>5.656854249492381E-2</v>
+      </c>
+      <c r="M9" s="108">
+        <f>L9/0.707*2</f>
+        <v>0.16002416547361759</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13">
+      <c r="C10" s="1"/>
+      <c r="D10" s="28">
+        <v>300</v>
+      </c>
+      <c r="E10" s="21">
+        <f t="shared" si="0"/>
+        <v>122.47448713915891</v>
+      </c>
+      <c r="F10" s="21">
+        <f>E10/0.707*2</f>
+        <v>346.46248129889369</v>
+      </c>
+      <c r="G10" s="21">
+        <f t="shared" si="1"/>
+        <v>2.4494897427831779</v>
+      </c>
+      <c r="H10" s="187">
+        <f t="shared" si="2"/>
+        <v>6.9292496259778726</v>
+      </c>
+      <c r="I10" s="188">
+        <f>E10/25</f>
+        <v>4.8989794855663567</v>
+      </c>
+      <c r="J10" s="21">
+        <f t="shared" si="3"/>
+        <v>13.858499251955749</v>
+      </c>
+      <c r="K10" s="189">
+        <f t="shared" si="4"/>
+        <v>0.48000000000000009</v>
+      </c>
+      <c r="L10" s="189">
+        <f t="shared" si="5"/>
+        <v>9.7979589711327128E-2</v>
+      </c>
+      <c r="M10" s="187">
+        <f t="shared" ref="M10:M12" si="6">L10/0.707*2</f>
+        <v>0.27716998503911494</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13">
+      <c r="C11" s="1"/>
+      <c r="D11" s="4">
+        <v>600</v>
+      </c>
+      <c r="E11" s="103">
+        <f t="shared" si="0"/>
+        <v>173.20508075688772</v>
+      </c>
+      <c r="F11" s="103">
+        <f>E11/0.707*2</f>
+        <v>489.97193990633025</v>
+      </c>
+      <c r="G11" s="103">
+        <f t="shared" si="1"/>
+        <v>3.4641016151377548</v>
+      </c>
+      <c r="H11" s="108">
+        <f t="shared" si="2"/>
+        <v>9.7994387981266051</v>
+      </c>
+      <c r="I11" s="171">
+        <f>E11/25</f>
+        <v>6.9282032302755088</v>
+      </c>
+      <c r="J11" s="103">
+        <f t="shared" si="3"/>
+        <v>19.598877596253207</v>
+      </c>
+      <c r="K11" s="172">
+        <f t="shared" si="4"/>
+        <v>0.95999999999999985</v>
+      </c>
+      <c r="L11" s="172">
+        <f t="shared" si="5"/>
+        <v>0.13856406460551016</v>
+      </c>
+      <c r="M11" s="108">
+        <f t="shared" si="6"/>
+        <v>0.39197755192506412</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" ht="18" thickBot="1">
+      <c r="C12" s="1"/>
+      <c r="D12" s="7">
+        <v>1000</v>
+      </c>
+      <c r="E12" s="173">
+        <f t="shared" si="0"/>
+        <v>223.60679774997897</v>
+      </c>
+      <c r="F12" s="173">
+        <f>E12/0.707*2</f>
+        <v>632.55105445538607</v>
+      </c>
+      <c r="G12" s="173">
+        <f t="shared" si="1"/>
+        <v>4.4721359549995796</v>
+      </c>
+      <c r="H12" s="186">
+        <f t="shared" si="2"/>
+        <v>12.651021089107722</v>
+      </c>
+      <c r="I12" s="174">
+        <f>E12/25</f>
+        <v>8.9442719099991592</v>
+      </c>
+      <c r="J12" s="173">
+        <f t="shared" si="3"/>
+        <v>25.302042178215444</v>
+      </c>
+      <c r="K12" s="175">
+        <f t="shared" si="4"/>
+        <v>1.6000000000000003</v>
+      </c>
+      <c r="L12" s="175">
+        <f t="shared" si="5"/>
+        <v>0.1788854381999832</v>
+      </c>
+      <c r="M12" s="186">
+        <f t="shared" si="6"/>
+        <v>0.5060408435643089</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" ht="18" thickBot="1">
+      <c r="D14" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" ht="18" thickBot="1">
+      <c r="D15" s="144" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="145"/>
+      <c r="F15" s="140" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15" s="205" t="s">
+        <v>161</v>
+      </c>
+      <c r="H15" s="142" t="s">
+        <v>49</v>
+      </c>
+      <c r="I15" s="142" t="s">
+        <v>162</v>
+      </c>
+      <c r="J15" s="205" t="s">
+        <v>161</v>
+      </c>
+      <c r="K15" s="205" t="s">
+        <v>161</v>
+      </c>
+      <c r="L15" s="141" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13">
+      <c r="D16" s="203" t="s">
+        <v>163</v>
+      </c>
+      <c r="E16" s="204"/>
+      <c r="F16" s="115">
+        <v>35.549999999999997</v>
+      </c>
+      <c r="G16" s="206">
+        <v>29</v>
+      </c>
+      <c r="H16" s="54">
+        <v>21</v>
+      </c>
+      <c r="I16" s="54">
+        <v>12.7</v>
+      </c>
+      <c r="J16" s="206">
+        <v>29</v>
+      </c>
+      <c r="K16" s="206">
+        <v>29</v>
+      </c>
+      <c r="L16" s="178" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="17" spans="3:18">
+      <c r="D17" s="176" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="177"/>
+      <c r="F17" s="4">
+        <v>885</v>
+      </c>
+      <c r="G17" s="19">
+        <v>510</v>
+      </c>
+      <c r="H17" s="2">
+        <v>470</v>
+      </c>
+      <c r="I17" s="2">
+        <v>440</v>
+      </c>
+      <c r="J17" s="19">
+        <v>510</v>
+      </c>
+      <c r="K17" s="19">
+        <v>510</v>
+      </c>
+      <c r="L17" s="5"/>
+    </row>
+    <row r="18" spans="3:18">
+      <c r="D18" s="176" t="s">
+        <v>165</v>
+      </c>
+      <c r="E18" s="177"/>
+      <c r="F18" s="179">
+        <f>F17*25^2/1000</f>
+        <v>553.125</v>
+      </c>
+      <c r="G18" s="21">
+        <f>G17*25^2/1000</f>
+        <v>318.75</v>
+      </c>
+      <c r="H18" s="103">
+        <f>H17*25^2/1000</f>
+        <v>293.75</v>
+      </c>
+      <c r="I18" s="103">
+        <f>I17*25^2/1000</f>
+        <v>275</v>
+      </c>
+      <c r="J18" s="21">
+        <f>J17*25^2/1000</f>
+        <v>318.75</v>
+      </c>
+      <c r="K18" s="21">
+        <f>K17*25^2/1000</f>
+        <v>318.75</v>
+      </c>
+      <c r="L18" s="5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="19" spans="3:18">
+      <c r="D19" s="176" t="s">
+        <v>167</v>
+      </c>
+      <c r="E19" s="177"/>
+      <c r="F19" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="G19" s="19">
+        <v>0.3</v>
+      </c>
+      <c r="H19" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="I19" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="J19" s="19">
+        <v>27.12</v>
+      </c>
+      <c r="K19" s="19">
+        <v>13.65</v>
+      </c>
+      <c r="L19" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="20" spans="3:18">
+      <c r="D20" s="176" t="s">
+        <v>169</v>
+      </c>
+      <c r="E20" s="177"/>
+      <c r="F20" s="179">
+        <f>2*3.14*F19*F18</f>
+        <v>1042.0874999999999</v>
+      </c>
+      <c r="G20" s="21">
+        <f>2*3.14*G19*G18</f>
+        <v>600.52499999999998</v>
+      </c>
+      <c r="H20" s="103">
+        <f>2*3.14*H19*H18</f>
+        <v>553.42499999999995</v>
+      </c>
+      <c r="I20" s="103">
+        <f>2*3.14*I19*I18</f>
+        <v>518.1</v>
+      </c>
+      <c r="J20" s="21">
+        <f>2*3.14*J19*J18</f>
+        <v>54287.46</v>
+      </c>
+      <c r="K20" s="21">
+        <f>2*3.14*K19*K18</f>
+        <v>27323.887500000004</v>
+      </c>
+      <c r="L20" s="180" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="21" spans="3:18" ht="18" thickBot="1">
+      <c r="D21" s="181" t="s">
+        <v>171</v>
+      </c>
+      <c r="E21" s="182"/>
+      <c r="F21" s="174">
+        <v>1.226</v>
+      </c>
+      <c r="G21" s="207">
+        <v>0.78</v>
+      </c>
+      <c r="H21" s="175">
+        <v>0.78</v>
+      </c>
+      <c r="I21" s="175">
+        <v>0.78</v>
+      </c>
+      <c r="J21" s="207">
+        <v>0.78</v>
+      </c>
+      <c r="K21" s="207">
+        <v>0.78</v>
+      </c>
+      <c r="L21" s="183" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="23" spans="3:18" ht="18" thickBot="1">
+      <c r="D23" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="24" spans="3:18">
+      <c r="D24" s="168" t="s">
+        <v>180</v>
+      </c>
+      <c r="E24" s="156"/>
+      <c r="F24" s="10">
+        <v>30</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="25" spans="3:18">
+      <c r="D25" s="176" t="s">
+        <v>181</v>
+      </c>
+      <c r="E25" s="184"/>
+      <c r="F25" s="2">
+        <f>300/F24</f>
+        <v>10</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="26" spans="3:18" ht="18" thickBot="1">
+      <c r="D26" s="181" t="s">
+        <v>182</v>
+      </c>
+      <c r="E26" s="208"/>
+      <c r="F26" s="8">
+        <f>F25/10</f>
+        <v>1</v>
+      </c>
+      <c r="G26" s="183" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="28" spans="3:18">
+      <c r="C28" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="29" spans="3:18" ht="18" thickBot="1">
+      <c r="C29" s="1"/>
+      <c r="D29" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="30" spans="3:18">
+      <c r="D30" s="212" t="s">
+        <v>177</v>
+      </c>
+      <c r="E30" s="213"/>
+      <c r="F30" s="213"/>
+      <c r="G30" s="213"/>
+      <c r="H30" s="237"/>
+      <c r="I30" s="212" t="s">
+        <v>192</v>
+      </c>
+      <c r="J30" s="213"/>
+      <c r="K30" s="213"/>
+      <c r="L30" s="196" t="s">
+        <v>187</v>
+      </c>
+      <c r="M30" s="197">
+        <v>25</v>
+      </c>
+      <c r="N30" s="190" t="s">
+        <v>183</v>
+      </c>
+      <c r="O30" s="198"/>
+      <c r="P30" s="190" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q30" s="191"/>
+      <c r="R30" s="192"/>
+    </row>
+    <row r="31" spans="3:18">
+      <c r="D31" s="214"/>
+      <c r="E31" s="210"/>
+      <c r="F31" s="210"/>
+      <c r="G31" s="210"/>
+      <c r="H31" s="238"/>
+      <c r="I31" s="214"/>
+      <c r="J31" s="210"/>
+      <c r="K31" s="210"/>
+      <c r="L31" s="211" t="s">
+        <v>188</v>
+      </c>
+      <c r="M31" s="241">
+        <v>1</v>
+      </c>
+      <c r="N31" s="209" t="s">
+        <v>189</v>
+      </c>
+      <c r="O31" s="246">
+        <v>1</v>
+      </c>
+      <c r="P31" s="209" t="s">
+        <v>191</v>
+      </c>
+      <c r="Q31" s="240">
+        <v>1</v>
+      </c>
+      <c r="R31" s="5"/>
+    </row>
+    <row r="32" spans="3:18" ht="18" thickBot="1">
+      <c r="D32" s="193" t="s">
+        <v>115</v>
+      </c>
+      <c r="E32" s="194" t="s">
+        <v>114</v>
+      </c>
+      <c r="F32" s="194" t="s">
+        <v>113</v>
+      </c>
+      <c r="G32" s="194" t="s">
+        <v>157</v>
+      </c>
+      <c r="H32" s="199" t="s">
+        <v>176</v>
+      </c>
+      <c r="I32" s="193" t="s">
+        <v>114</v>
+      </c>
+      <c r="J32" s="194" t="s">
+        <v>113</v>
+      </c>
+      <c r="K32" s="194" t="s">
+        <v>115</v>
+      </c>
+      <c r="L32" s="194" t="s">
+        <v>157</v>
+      </c>
+      <c r="M32" s="195" t="s">
+        <v>176</v>
+      </c>
+      <c r="N32" s="193" t="s">
+        <v>114</v>
+      </c>
+      <c r="O32" s="199" t="s">
+        <v>115</v>
+      </c>
+      <c r="P32" s="193" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q32" s="194" t="s">
+        <v>115</v>
+      </c>
+      <c r="R32" s="195" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="33" spans="4:18">
+      <c r="D33" s="219">
+        <v>50</v>
+      </c>
+      <c r="E33" s="220">
+        <f>(D33*50)^0.5</f>
+        <v>50</v>
+      </c>
+      <c r="F33" s="220">
+        <f>E33/0.707*2</f>
+        <v>141.44271570014146</v>
+      </c>
+      <c r="G33" s="220">
+        <f>D33/E33</f>
+        <v>1</v>
+      </c>
+      <c r="H33" s="221">
+        <f>G33/0.707*2</f>
+        <v>2.8288543140028288</v>
+      </c>
+      <c r="I33" s="251">
+        <f>E33/M$30</f>
+        <v>2</v>
+      </c>
+      <c r="J33" s="220">
+        <f>I33/0.707*2</f>
+        <v>5.6577086280056577</v>
+      </c>
+      <c r="K33" s="220">
+        <f>I33*I33/50</f>
+        <v>0.08</v>
+      </c>
+      <c r="L33" s="222">
+        <f>K33/I33</f>
+        <v>0.04</v>
+      </c>
+      <c r="M33" s="221">
+        <f>L33/0.707*2</f>
+        <v>0.11315417256011316</v>
+      </c>
+      <c r="N33" s="242">
+        <f>I33*O$31/(O$31+Q$31)</f>
+        <v>1</v>
+      </c>
+      <c r="O33" s="247">
+        <f>N33*N33/(O$31*1000)</f>
+        <v>1E-3</v>
+      </c>
+      <c r="P33" s="251">
+        <f>I33*Q$31/(O$31+Q$31)</f>
+        <v>1</v>
+      </c>
+      <c r="Q33" s="223">
+        <f>P33*P33/(Q$31*1000)</f>
+        <v>1E-3</v>
+      </c>
+      <c r="R33" s="221">
+        <f>P33/0.707*2</f>
+        <v>2.8288543140028288</v>
+      </c>
+    </row>
+    <row r="34" spans="4:18">
+      <c r="D34" s="225">
+        <v>100</v>
+      </c>
+      <c r="E34" s="226">
+        <f t="shared" ref="E34:E35" si="7">(D34*50)^0.5</f>
+        <v>70.710678118654755</v>
+      </c>
+      <c r="F34" s="226">
+        <f>E34/0.707*2</f>
+        <v>200.03020684202195</v>
+      </c>
+      <c r="G34" s="226">
+        <f t="shared" ref="G34:G35" si="8">D34/E34</f>
+        <v>1.4142135623730949</v>
+      </c>
+      <c r="H34" s="227">
+        <f t="shared" ref="H34:H39" si="9">G34/0.707*2</f>
+        <v>4.0006041368404386</v>
+      </c>
+      <c r="I34" s="242">
+        <f t="shared" ref="I34:I39" si="10">E34/M$30</f>
+        <v>2.8284271247461903</v>
+      </c>
+      <c r="J34" s="239">
+        <f t="shared" ref="J34:J39" si="11">I34/0.707*2</f>
+        <v>8.0012082736808789</v>
+      </c>
+      <c r="K34" s="226">
+        <f t="shared" ref="K34:K35" si="12">I34*I34/50</f>
+        <v>0.16000000000000003</v>
+      </c>
+      <c r="L34" s="228">
+        <f t="shared" ref="L34:L35" si="13">K34/I34</f>
+        <v>5.656854249492381E-2</v>
+      </c>
+      <c r="M34" s="227">
+        <f>L34/0.707*2</f>
+        <v>0.16002416547361759</v>
+      </c>
+      <c r="N34" s="243">
+        <f>I34*O$31/(O$31+Q$31)</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="O34" s="248">
+        <f>N34*N34/(O$31*1000)</f>
+        <v>2.0000000000000005E-3</v>
+      </c>
+      <c r="P34" s="243">
+        <f>I34*Q$31/(O$31+Q$31)</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="Q34" s="229">
+        <f>P34*P34/(Q$31*1000)</f>
+        <v>2.0000000000000005E-3</v>
+      </c>
+      <c r="R34" s="227">
+        <f t="shared" ref="R34:R39" si="14">P34/0.707*2</f>
+        <v>4.0006041368404395</v>
+      </c>
+    </row>
+    <row r="35" spans="4:18">
+      <c r="D35" s="225">
+        <v>150</v>
+      </c>
+      <c r="E35" s="226">
+        <f t="shared" si="7"/>
+        <v>86.602540378443862</v>
+      </c>
+      <c r="F35" s="226">
+        <f>E35/0.707*2</f>
+        <v>244.98596995316512</v>
+      </c>
+      <c r="G35" s="226">
+        <f t="shared" si="8"/>
+        <v>1.7320508075688774</v>
+      </c>
+      <c r="H35" s="227">
+        <f t="shared" si="9"/>
+        <v>4.8997193990633026</v>
+      </c>
+      <c r="I35" s="242">
+        <f t="shared" si="10"/>
+        <v>3.4641016151377544</v>
+      </c>
+      <c r="J35" s="239">
+        <f t="shared" si="11"/>
+        <v>9.7994387981266033</v>
+      </c>
+      <c r="K35" s="226">
+        <f t="shared" si="12"/>
+        <v>0.23999999999999996</v>
+      </c>
+      <c r="L35" s="228">
+        <f t="shared" si="13"/>
+        <v>6.9282032302755078E-2</v>
+      </c>
+      <c r="M35" s="227">
+        <f t="shared" ref="M35:M39" si="15">L35/0.707*2</f>
+        <v>0.19598877596253206</v>
+      </c>
+      <c r="N35" s="243">
+        <f>I35*O$31/(O$31+Q$31)</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="O35" s="248">
+        <f>N35*N35/(O$31*1000)</f>
+        <v>2.9999999999999996E-3</v>
+      </c>
+      <c r="P35" s="243">
+        <f>I35*Q$31/(O$31+Q$31)</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="Q35" s="229">
+        <f>P35*P35/(Q$31*1000)</f>
+        <v>2.9999999999999996E-3</v>
+      </c>
+      <c r="R35" s="227">
+        <f t="shared" si="14"/>
+        <v>4.8997193990633017</v>
+      </c>
+    </row>
+    <row r="36" spans="4:18">
+      <c r="D36" s="225">
+        <v>200</v>
+      </c>
+      <c r="E36" s="226">
+        <f t="shared" ref="E36" si="16">(D36*50)^0.5</f>
+        <v>100</v>
+      </c>
+      <c r="F36" s="226">
+        <f>E36/0.707*2</f>
+        <v>282.88543140028293</v>
+      </c>
+      <c r="G36" s="226">
+        <f t="shared" ref="G36" si="17">D36/E36</f>
+        <v>2</v>
+      </c>
+      <c r="H36" s="227">
+        <f t="shared" si="9"/>
+        <v>5.6577086280056577</v>
+      </c>
+      <c r="I36" s="242">
+        <f t="shared" si="10"/>
+        <v>4</v>
+      </c>
+      <c r="J36" s="239">
+        <f t="shared" si="11"/>
+        <v>11.315417256011315</v>
+      </c>
+      <c r="K36" s="226">
+        <f t="shared" ref="K36" si="18">I36*I36/50</f>
+        <v>0.32</v>
+      </c>
+      <c r="L36" s="228">
+        <f t="shared" ref="L36" si="19">K36/I36</f>
+        <v>0.08</v>
+      </c>
+      <c r="M36" s="227">
+        <f t="shared" si="15"/>
+        <v>0.22630834512022632</v>
+      </c>
+      <c r="N36" s="243">
+        <f>I36*O$31/(O$31+Q$31)</f>
+        <v>2</v>
+      </c>
+      <c r="O36" s="248">
+        <f>N36*N36/(O$31*1000)</f>
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="P36" s="243">
+        <f>I36*Q$31/(O$31+Q$31)</f>
+        <v>2</v>
+      </c>
+      <c r="Q36" s="229">
+        <f>P36*P36/(Q$31*1000)</f>
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="R36" s="227">
+        <f t="shared" si="14"/>
+        <v>5.6577086280056577</v>
+      </c>
+    </row>
+    <row r="37" spans="4:18">
+      <c r="D37" s="225">
+        <v>250</v>
+      </c>
+      <c r="E37" s="226">
+        <f t="shared" ref="E37" si="20">(D37*50)^0.5</f>
+        <v>111.80339887498948</v>
+      </c>
+      <c r="F37" s="226">
+        <f>E37/0.707*2</f>
+        <v>316.27552722769303</v>
+      </c>
+      <c r="G37" s="226">
+        <f t="shared" ref="G37" si="21">D37/E37</f>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="H37" s="227">
+        <f t="shared" si="9"/>
+        <v>6.3255105445538611</v>
+      </c>
+      <c r="I37" s="242">
+        <f t="shared" si="10"/>
+        <v>4.4721359549995796</v>
+      </c>
+      <c r="J37" s="239">
+        <f t="shared" si="11"/>
+        <v>12.651021089107722</v>
+      </c>
+      <c r="K37" s="226">
+        <f t="shared" ref="K37" si="22">I37*I37/50</f>
+        <v>0.40000000000000008</v>
+      </c>
+      <c r="L37" s="228">
+        <f t="shared" ref="L37" si="23">K37/I37</f>
+        <v>8.9442719099991602E-2</v>
+      </c>
+      <c r="M37" s="227">
+        <f t="shared" si="15"/>
+        <v>0.25302042178215445</v>
+      </c>
+      <c r="N37" s="243">
+        <f>I37*O$31/(O$31+Q$31)</f>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="O37" s="248">
+        <f>N37*N37/(O$31*1000)</f>
+        <v>5.000000000000001E-3</v>
+      </c>
+      <c r="P37" s="243">
+        <f>I37*Q$31/(O$31+Q$31)</f>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="Q37" s="229">
+        <f>P37*P37/(Q$31*1000)</f>
+        <v>5.000000000000001E-3</v>
+      </c>
+      <c r="R37" s="227">
+        <f t="shared" si="14"/>
+        <v>6.3255105445538611</v>
+      </c>
+    </row>
+    <row r="38" spans="4:18">
+      <c r="D38" s="225">
+        <v>300</v>
+      </c>
+      <c r="E38" s="226">
+        <f t="shared" ref="E38:E39" si="24">(D38*50)^0.5</f>
+        <v>122.47448713915891</v>
+      </c>
+      <c r="F38" s="226">
+        <f>E38/0.707*2</f>
+        <v>346.46248129889369</v>
+      </c>
+      <c r="G38" s="226">
+        <f t="shared" ref="G38:G39" si="25">D38/E38</f>
+        <v>2.4494897427831779</v>
+      </c>
+      <c r="H38" s="227">
+        <f t="shared" si="9"/>
+        <v>6.9292496259778726</v>
+      </c>
+      <c r="I38" s="242">
+        <f t="shared" si="10"/>
+        <v>4.8989794855663567</v>
+      </c>
+      <c r="J38" s="239">
+        <f t="shared" si="11"/>
+        <v>13.858499251955749</v>
+      </c>
+      <c r="K38" s="226">
+        <f t="shared" ref="K38:K39" si="26">I38*I38/50</f>
+        <v>0.48000000000000009</v>
+      </c>
+      <c r="L38" s="228">
+        <f t="shared" ref="L38:L39" si="27">K38/I38</f>
+        <v>9.7979589711327128E-2</v>
+      </c>
+      <c r="M38" s="227">
+        <f t="shared" si="15"/>
+        <v>0.27716998503911494</v>
+      </c>
+      <c r="N38" s="243">
+        <f>I38*O$31/(O$31+Q$31)</f>
+        <v>2.4494897427831783</v>
+      </c>
+      <c r="O38" s="248">
+        <f>N38*N38/(O$31*1000)</f>
+        <v>6.000000000000001E-3</v>
+      </c>
+      <c r="P38" s="243">
+        <f>I38*Q$31/(O$31+Q$31)</f>
+        <v>2.4494897427831783</v>
+      </c>
+      <c r="Q38" s="229">
+        <f>P38*P38/(Q$31*1000)</f>
+        <v>6.000000000000001E-3</v>
+      </c>
+      <c r="R38" s="227">
+        <f t="shared" si="14"/>
+        <v>6.9292496259778744</v>
+      </c>
+    </row>
+    <row r="39" spans="4:18" ht="18" thickBot="1">
+      <c r="D39" s="231">
+        <v>350</v>
+      </c>
+      <c r="E39" s="232">
+        <f t="shared" si="24"/>
+        <v>132.28756555322954</v>
+      </c>
+      <c r="F39" s="232">
+        <f>E39/0.707*2</f>
+        <v>374.22225050418541</v>
+      </c>
+      <c r="G39" s="232">
+        <f t="shared" si="25"/>
+        <v>2.6457513110645903</v>
+      </c>
+      <c r="H39" s="233">
+        <f t="shared" si="9"/>
+        <v>7.4844450100837072</v>
+      </c>
+      <c r="I39" s="252">
+        <f t="shared" si="10"/>
+        <v>5.2915026221291814</v>
+      </c>
+      <c r="J39" s="245">
+        <f t="shared" si="11"/>
+        <v>14.968890020167416</v>
+      </c>
+      <c r="K39" s="232">
+        <f t="shared" si="26"/>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="L39" s="234">
+        <f t="shared" si="27"/>
+        <v>0.10583005244258363</v>
+      </c>
+      <c r="M39" s="233">
+        <f t="shared" si="15"/>
+        <v>0.29937780040334833</v>
+      </c>
+      <c r="N39" s="244">
+        <f>I39*O$31/(O$31+Q$31)</f>
+        <v>2.6457513110645907</v>
+      </c>
+      <c r="O39" s="249">
+        <f>N39*N39/(O$31*1000)</f>
+        <v>7.000000000000001E-3</v>
+      </c>
+      <c r="P39" s="244">
+        <f>I39*Q$31/(O$31+Q$31)</f>
+        <v>2.6457513110645907</v>
+      </c>
+      <c r="Q39" s="235">
+        <f>P39*P39/(Q$31*1000)</f>
+        <v>7.000000000000001E-3</v>
+      </c>
+      <c r="R39" s="233">
+        <f t="shared" si="14"/>
+        <v>7.4844450100837081</v>
+      </c>
+    </row>
+    <row r="40" spans="4:18">
+      <c r="D40" s="257"/>
+      <c r="E40" s="258"/>
+      <c r="F40" s="258"/>
+      <c r="G40" s="258"/>
+      <c r="H40" s="258"/>
+      <c r="I40" s="259"/>
+      <c r="J40" s="258"/>
+      <c r="K40" s="258"/>
+      <c r="L40" s="259"/>
+      <c r="M40" s="258"/>
+      <c r="N40" s="259"/>
+      <c r="O40" s="260"/>
+      <c r="P40" s="259"/>
+      <c r="Q40" s="260"/>
+      <c r="R40" s="258"/>
+    </row>
+    <row r="41" spans="4:18" ht="18" thickBot="1">
+      <c r="D41" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="42" spans="4:18">
+      <c r="D42" s="212" t="s">
+        <v>177</v>
+      </c>
+      <c r="E42" s="213"/>
+      <c r="F42" s="213"/>
+      <c r="G42" s="213"/>
+      <c r="H42" s="217"/>
+      <c r="I42" s="215" t="s">
+        <v>193</v>
+      </c>
+      <c r="J42" s="213"/>
+      <c r="K42" s="213"/>
+      <c r="L42" s="196" t="s">
+        <v>187</v>
+      </c>
+      <c r="M42" s="197">
+        <v>1</v>
+      </c>
+      <c r="N42" s="190" t="s">
+        <v>183</v>
+      </c>
+      <c r="O42" s="198"/>
+      <c r="P42" s="190" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q42" s="191"/>
+      <c r="R42" s="192"/>
+    </row>
+    <row r="43" spans="4:18">
+      <c r="D43" s="214"/>
+      <c r="E43" s="210"/>
+      <c r="F43" s="210"/>
+      <c r="G43" s="210"/>
+      <c r="H43" s="218"/>
+      <c r="I43" s="216"/>
+      <c r="J43" s="210"/>
+      <c r="K43" s="210"/>
+      <c r="L43" s="211" t="s">
+        <v>188</v>
+      </c>
+      <c r="M43" s="241">
+        <v>25</v>
+      </c>
+      <c r="N43" s="209" t="s">
+        <v>189</v>
+      </c>
+      <c r="O43" s="246">
+        <v>1</v>
+      </c>
+      <c r="P43" s="209" t="s">
+        <v>190</v>
+      </c>
+      <c r="Q43" s="240">
+        <v>1</v>
+      </c>
+      <c r="R43" s="5"/>
+    </row>
+    <row r="44" spans="4:18" ht="18" thickBot="1">
+      <c r="D44" s="193" t="s">
+        <v>115</v>
+      </c>
+      <c r="E44" s="194" t="s">
+        <v>114</v>
+      </c>
+      <c r="F44" s="194" t="s">
+        <v>113</v>
+      </c>
+      <c r="G44" s="194" t="s">
+        <v>157</v>
+      </c>
+      <c r="H44" s="195" t="s">
+        <v>176</v>
+      </c>
+      <c r="I44" s="250" t="s">
+        <v>157</v>
+      </c>
+      <c r="J44" s="202" t="s">
+        <v>176</v>
+      </c>
+      <c r="K44" s="200" t="s">
+        <v>114</v>
+      </c>
+      <c r="L44" s="201" t="s">
+        <v>113</v>
+      </c>
+      <c r="M44" s="201" t="s">
+        <v>115</v>
+      </c>
+      <c r="N44" s="200" t="s">
+        <v>114</v>
+      </c>
+      <c r="O44" s="256" t="s">
+        <v>115</v>
+      </c>
+      <c r="P44" s="200" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q44" s="201" t="s">
+        <v>115</v>
+      </c>
+      <c r="R44" s="202" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="45" spans="4:18">
+      <c r="D45" s="219">
+        <v>50</v>
+      </c>
+      <c r="E45" s="220">
+        <f>(D45*50)^0.5</f>
+        <v>50</v>
+      </c>
+      <c r="F45" s="220">
+        <f>E45/0.707*2</f>
+        <v>141.44271570014146</v>
+      </c>
+      <c r="G45" s="220">
+        <f>D45/E45</f>
+        <v>1</v>
+      </c>
+      <c r="H45" s="253">
+        <f>G45/0.707*2</f>
+        <v>2.8288543140028288</v>
+      </c>
+      <c r="I45" s="251">
+        <f>G45/M$43</f>
+        <v>0.04</v>
+      </c>
+      <c r="J45" s="220">
+        <f>I45/0.707*2</f>
+        <v>0.11315417256011316</v>
+      </c>
+      <c r="K45" s="222">
+        <f>I45*50</f>
+        <v>2</v>
+      </c>
+      <c r="L45" s="220">
+        <f>K45/0.707*2</f>
+        <v>5.6577086280056577</v>
+      </c>
+      <c r="M45" s="221">
+        <f>I45*K45</f>
+        <v>0.08</v>
+      </c>
+      <c r="N45" s="251">
+        <f>K45*O$31/(O$31+Q$31)</f>
+        <v>1</v>
+      </c>
+      <c r="O45" s="224">
+        <f>N45*N45/(O$31*1000)</f>
+        <v>1E-3</v>
+      </c>
+      <c r="P45" s="251">
+        <f>K45*Q$31/(O$31+Q$31)</f>
+        <v>1</v>
+      </c>
+      <c r="Q45" s="223">
+        <f>P45*P45/(Q$31*1000)</f>
+        <v>1E-3</v>
+      </c>
+      <c r="R45" s="221">
+        <f>P45/0.707*2</f>
+        <v>2.8288543140028288</v>
+      </c>
+    </row>
+    <row r="46" spans="4:18">
+      <c r="D46" s="225">
+        <v>100</v>
+      </c>
+      <c r="E46" s="226">
+        <f t="shared" ref="E46:E51" si="28">(D46*50)^0.5</f>
+        <v>70.710678118654755</v>
+      </c>
+      <c r="F46" s="226">
+        <f>E46/0.707*2</f>
+        <v>200.03020684202195</v>
+      </c>
+      <c r="G46" s="226">
+        <f t="shared" ref="G46:G51" si="29">D46/E46</f>
+        <v>1.4142135623730949</v>
+      </c>
+      <c r="H46" s="254">
+        <f t="shared" ref="H46:H51" si="30">G46/0.707*2</f>
+        <v>4.0006041368404386</v>
+      </c>
+      <c r="I46" s="243">
+        <f t="shared" ref="I46:I51" si="31">G46/M$43</f>
+        <v>5.6568542494923796E-2</v>
+      </c>
+      <c r="J46" s="226">
+        <f t="shared" ref="J46:J51" si="32">I46/0.707*2</f>
+        <v>0.16002416547361753</v>
+      </c>
+      <c r="K46" s="228">
+        <f t="shared" ref="K46:K51" si="33">I46*50</f>
+        <v>2.8284271247461898</v>
+      </c>
+      <c r="L46" s="226">
+        <f t="shared" ref="L46:L51" si="34">K46/0.707*2</f>
+        <v>8.0012082736808772</v>
+      </c>
+      <c r="M46" s="227">
+        <f t="shared" ref="M46:M51" si="35">I46*K46</f>
+        <v>0.15999999999999998</v>
+      </c>
+      <c r="N46" s="243">
+        <f t="shared" ref="N46:N51" si="36">K46*O$31/(O$31+Q$31)</f>
+        <v>1.4142135623730949</v>
+      </c>
+      <c r="O46" s="230">
+        <f>N46*N46/(O$31*1000)</f>
+        <v>1.9999999999999996E-3</v>
+      </c>
+      <c r="P46" s="243">
+        <f t="shared" ref="P46:P51" si="37">K46*Q$31/(O$31+Q$31)</f>
+        <v>1.4142135623730949</v>
+      </c>
+      <c r="Q46" s="229">
+        <f>P46*P46/(Q$31*1000)</f>
+        <v>1.9999999999999996E-3</v>
+      </c>
+      <c r="R46" s="227">
+        <f t="shared" ref="R46:R51" si="38">P46/0.707*2</f>
+        <v>4.0006041368404386</v>
+      </c>
+    </row>
+    <row r="47" spans="4:18">
+      <c r="D47" s="225">
+        <v>150</v>
+      </c>
+      <c r="E47" s="226">
+        <f t="shared" si="28"/>
+        <v>86.602540378443862</v>
+      </c>
+      <c r="F47" s="226">
+        <f>E47/0.707*2</f>
+        <v>244.98596995316512</v>
+      </c>
+      <c r="G47" s="226">
+        <f t="shared" si="29"/>
+        <v>1.7320508075688774</v>
+      </c>
+      <c r="H47" s="254">
+        <f t="shared" si="30"/>
+        <v>4.8997193990633026</v>
+      </c>
+      <c r="I47" s="243">
+        <f t="shared" si="31"/>
+        <v>6.9282032302755092E-2</v>
+      </c>
+      <c r="J47" s="226">
+        <f t="shared" si="32"/>
+        <v>0.19598877596253209</v>
+      </c>
+      <c r="K47" s="228">
+        <f t="shared" si="33"/>
+        <v>3.4641016151377544</v>
+      </c>
+      <c r="L47" s="226">
+        <f t="shared" si="34"/>
+        <v>9.7994387981266033</v>
+      </c>
+      <c r="M47" s="227">
+        <f t="shared" si="35"/>
+        <v>0.24</v>
+      </c>
+      <c r="N47" s="243">
+        <f t="shared" si="36"/>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="O47" s="230">
+        <f>N47*N47/(O$31*1000)</f>
+        <v>2.9999999999999996E-3</v>
+      </c>
+      <c r="P47" s="243">
+        <f t="shared" si="37"/>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="Q47" s="229">
+        <f>P47*P47/(Q$31*1000)</f>
+        <v>2.9999999999999996E-3</v>
+      </c>
+      <c r="R47" s="227">
+        <f t="shared" si="38"/>
+        <v>4.8997193990633017</v>
+      </c>
+    </row>
+    <row r="48" spans="4:18">
+      <c r="D48" s="225">
+        <v>200</v>
+      </c>
+      <c r="E48" s="226">
+        <f t="shared" si="28"/>
+        <v>100</v>
+      </c>
+      <c r="F48" s="226">
+        <f>E48/0.707*2</f>
+        <v>282.88543140028293</v>
+      </c>
+      <c r="G48" s="226">
+        <f t="shared" si="29"/>
+        <v>2</v>
+      </c>
+      <c r="H48" s="254">
+        <f t="shared" si="30"/>
+        <v>5.6577086280056577</v>
+      </c>
+      <c r="I48" s="243">
+        <f t="shared" si="31"/>
+        <v>0.08</v>
+      </c>
+      <c r="J48" s="226">
+        <f t="shared" si="32"/>
+        <v>0.22630834512022632</v>
+      </c>
+      <c r="K48" s="228">
+        <f t="shared" si="33"/>
+        <v>4</v>
+      </c>
+      <c r="L48" s="226">
+        <f t="shared" si="34"/>
+        <v>11.315417256011315</v>
+      </c>
+      <c r="M48" s="227">
+        <f t="shared" si="35"/>
+        <v>0.32</v>
+      </c>
+      <c r="N48" s="243">
+        <f t="shared" si="36"/>
+        <v>2</v>
+      </c>
+      <c r="O48" s="230">
+        <f>N48*N48/(O$31*1000)</f>
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="P48" s="243">
+        <f t="shared" si="37"/>
+        <v>2</v>
+      </c>
+      <c r="Q48" s="229">
+        <f>P48*P48/(Q$31*1000)</f>
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="R48" s="227">
+        <f t="shared" si="38"/>
+        <v>5.6577086280056577</v>
+      </c>
+    </row>
+    <row r="49" spans="4:18">
+      <c r="D49" s="225">
+        <v>250</v>
+      </c>
+      <c r="E49" s="226">
+        <f t="shared" si="28"/>
+        <v>111.80339887498948</v>
+      </c>
+      <c r="F49" s="226">
+        <f>E49/0.707*2</f>
+        <v>316.27552722769303</v>
+      </c>
+      <c r="G49" s="226">
+        <f t="shared" si="29"/>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="H49" s="254">
+        <f t="shared" si="30"/>
+        <v>6.3255105445538611</v>
+      </c>
+      <c r="I49" s="243">
+        <f t="shared" si="31"/>
+        <v>8.9442719099991588E-2</v>
+      </c>
+      <c r="J49" s="226">
+        <f t="shared" si="32"/>
+        <v>0.25302042178215445</v>
+      </c>
+      <c r="K49" s="228">
+        <f t="shared" si="33"/>
+        <v>4.4721359549995796</v>
+      </c>
+      <c r="L49" s="226">
+        <f t="shared" si="34"/>
+        <v>12.651021089107722</v>
+      </c>
+      <c r="M49" s="227">
+        <f t="shared" si="35"/>
+        <v>0.4</v>
+      </c>
+      <c r="N49" s="243">
+        <f t="shared" si="36"/>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="O49" s="230">
+        <f>N49*N49/(O$31*1000)</f>
+        <v>5.000000000000001E-3</v>
+      </c>
+      <c r="P49" s="243">
+        <f t="shared" si="37"/>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="Q49" s="229">
+        <f>P49*P49/(Q$31*1000)</f>
+        <v>5.000000000000001E-3</v>
+      </c>
+      <c r="R49" s="227">
+        <f t="shared" si="38"/>
+        <v>6.3255105445538611</v>
+      </c>
+    </row>
+    <row r="50" spans="4:18">
+      <c r="D50" s="225">
+        <v>300</v>
+      </c>
+      <c r="E50" s="226">
+        <f t="shared" si="28"/>
+        <v>122.47448713915891</v>
+      </c>
+      <c r="F50" s="226">
+        <f>E50/0.707*2</f>
+        <v>346.46248129889369</v>
+      </c>
+      <c r="G50" s="226">
+        <f t="shared" si="29"/>
+        <v>2.4494897427831779</v>
+      </c>
+      <c r="H50" s="254">
+        <f t="shared" si="30"/>
+        <v>6.9292496259778726</v>
+      </c>
+      <c r="I50" s="243">
+        <f t="shared" si="31"/>
+        <v>9.7979589711327114E-2</v>
+      </c>
+      <c r="J50" s="226">
+        <f t="shared" si="32"/>
+        <v>0.27716998503911489</v>
+      </c>
+      <c r="K50" s="228">
+        <f t="shared" si="33"/>
+        <v>4.8989794855663558</v>
+      </c>
+      <c r="L50" s="226">
+        <f t="shared" si="34"/>
+        <v>13.858499251955745</v>
+      </c>
+      <c r="M50" s="227">
+        <f t="shared" si="35"/>
+        <v>0.47999999999999993</v>
+      </c>
+      <c r="N50" s="243">
+        <f t="shared" si="36"/>
+        <v>2.4494897427831779</v>
+      </c>
+      <c r="O50" s="230">
+        <f>N50*N50/(O$31*1000)</f>
+        <v>5.9999999999999993E-3</v>
+      </c>
+      <c r="P50" s="243">
+        <f t="shared" si="37"/>
+        <v>2.4494897427831779</v>
+      </c>
+      <c r="Q50" s="229">
+        <f>P50*P50/(Q$31*1000)</f>
+        <v>5.9999999999999993E-3</v>
+      </c>
+      <c r="R50" s="227">
+        <f t="shared" si="38"/>
+        <v>6.9292496259778726</v>
+      </c>
+    </row>
+    <row r="51" spans="4:18" ht="18" thickBot="1">
+      <c r="D51" s="231">
+        <v>350</v>
+      </c>
+      <c r="E51" s="232">
+        <f t="shared" si="28"/>
+        <v>132.28756555322954</v>
+      </c>
+      <c r="F51" s="232">
+        <f>E51/0.707*2</f>
+        <v>374.22225050418541</v>
+      </c>
+      <c r="G51" s="232">
+        <f t="shared" si="29"/>
+        <v>2.6457513110645903</v>
+      </c>
+      <c r="H51" s="255">
+        <f t="shared" si="30"/>
+        <v>7.4844450100837072</v>
+      </c>
+      <c r="I51" s="244">
+        <f t="shared" si="31"/>
+        <v>0.10583005244258362</v>
+      </c>
+      <c r="J51" s="232">
+        <f t="shared" si="32"/>
+        <v>0.29937780040334827</v>
+      </c>
+      <c r="K51" s="234">
+        <f t="shared" si="33"/>
+        <v>5.2915026221291805</v>
+      </c>
+      <c r="L51" s="232">
+        <f t="shared" si="34"/>
+        <v>14.968890020167414</v>
+      </c>
+      <c r="M51" s="233">
+        <f t="shared" si="35"/>
+        <v>0.55999999999999994</v>
+      </c>
+      <c r="N51" s="244">
+        <f t="shared" si="36"/>
+        <v>2.6457513110645903</v>
+      </c>
+      <c r="O51" s="236">
+        <f>N51*N51/(O$31*1000)</f>
+        <v>6.9999999999999984E-3</v>
+      </c>
+      <c r="P51" s="244">
+        <f t="shared" si="37"/>
+        <v>2.6457513110645903</v>
+      </c>
+      <c r="Q51" s="235">
+        <f>P51*P51/(Q$31*1000)</f>
+        <v>6.9999999999999984E-3</v>
+      </c>
+      <c r="R51" s="233">
+        <f t="shared" si="38"/>
+        <v>7.4844450100837072</v>
+      </c>
+    </row>
+    <row r="53" spans="4:18" ht="18" thickBot="1">
+      <c r="D53" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="54" spans="4:18">
+      <c r="D54" s="265" t="s">
+        <v>197</v>
+      </c>
+      <c r="E54" s="3">
+        <v>1</v>
+      </c>
+      <c r="F54" s="10">
+        <v>1</v>
+      </c>
+      <c r="G54" s="11">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="H54" s="262" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="55" spans="4:18">
+      <c r="D55" s="266" t="s">
+        <v>198</v>
+      </c>
+      <c r="E55" s="4">
+        <v>100</v>
+      </c>
+      <c r="F55" s="2">
+        <v>47</v>
+      </c>
+      <c r="G55" s="5">
+        <v>100</v>
+      </c>
+      <c r="H55" s="263" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="56" spans="4:18">
+      <c r="D56" s="266" t="s">
+        <v>200</v>
+      </c>
+      <c r="E56" s="4">
+        <f>(1/(2*3.14*E54*1000*E55*10^(-12)))/1000</f>
+        <v>1592.3566878980891</v>
+      </c>
+      <c r="F56" s="2">
+        <f>(1/(2*3.14*F54*1000*F55*10^(-12)))/1000</f>
+        <v>3387.9929529746578</v>
+      </c>
+      <c r="G56" s="5">
+        <f>(1/(2*3.14*G54*1000*G55*10^(-12)))/1000</f>
+        <v>2843.4940855323021</v>
+      </c>
+      <c r="H56" s="263" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="57" spans="4:18" ht="18" thickBot="1">
+      <c r="D57" s="267" t="s">
+        <v>202</v>
+      </c>
+      <c r="E57" s="7">
+        <f>1/(2*3.14*E56)*1000</f>
+        <v>0.1</v>
+      </c>
+      <c r="F57" s="8">
+        <f>1/(2*3.14*F56)*1000</f>
+        <v>4.7E-2</v>
+      </c>
+      <c r="G57" s="9">
+        <f>1/(2*3.14*G56)*1000</f>
+        <v>5.5999999999999994E-2</v>
+      </c>
+      <c r="H57" s="264" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="59" spans="4:18" ht="18" thickBot="1">
+      <c r="D59" s="261" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="60" spans="4:18">
+      <c r="D60" s="265" t="s">
+        <v>198</v>
+      </c>
+      <c r="E60" s="3">
+        <v>20</v>
+      </c>
+      <c r="F60" s="10">
+        <v>68</v>
+      </c>
+      <c r="G60" s="10">
+        <v>100</v>
+      </c>
+      <c r="H60" s="11">
+        <v>100000</v>
+      </c>
+      <c r="I60" s="262" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="61" spans="4:18">
+      <c r="D61" s="266" t="s">
+        <v>200</v>
+      </c>
+      <c r="E61" s="4">
+        <v>27120</v>
+      </c>
+      <c r="F61" s="2">
+        <v>13560</v>
+      </c>
+      <c r="G61" s="2">
+        <v>13560</v>
+      </c>
+      <c r="H61" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="I61" s="263" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="62" spans="4:18" ht="18" thickBot="1">
+      <c r="D62" s="268" t="s">
+        <v>205</v>
+      </c>
+      <c r="E62" s="7">
+        <f>(1/(2*3.14*E61*1000*E60*10^(-12)))</f>
+        <v>293.57608552693381</v>
+      </c>
+      <c r="F62" s="8">
+        <f>(1/(2*3.14*F61*1000*F60*10^(-12)))</f>
+        <v>172.69181501584345</v>
+      </c>
+      <c r="G62" s="8">
+        <f>(1/(2*3.14*G61*1000*G60*10^(-12)))</f>
+        <v>117.43043421077354</v>
+      </c>
+      <c r="H62" s="9">
+        <f>(1/(2*3.14*H61*1000*H60*10^(-12)))</f>
+        <v>1990.4458598726112</v>
+      </c>
+      <c r="I62" s="264" t="s">
+        <v>170</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="20">
+    <mergeCell ref="N42:O42"/>
+    <mergeCell ref="P42:R42"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="D30:H31"/>
+    <mergeCell ref="I30:K31"/>
+    <mergeCell ref="P30:R30"/>
+    <mergeCell ref="D42:H43"/>
+    <mergeCell ref="I42:K43"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="I6:M6"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="G8:G12" formula="1"/>
+  </ignoredErrors>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <sheetData>
-    <row r="2" spans="2:8" ht="17.25" thickBot="1"/>
-    <row r="3" spans="2:8" ht="17.25" thickBot="1">
+    <row r="2" spans="2:8" ht="18" thickBot="1"/>
+    <row r="3" spans="2:8" ht="18" thickBot="1">
       <c r="B3" s="52" t="s">
         <v>84</v>
       </c>
@@ -2985,7 +5691,7 @@
       </c>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="2:8" ht="17.25" thickBot="1">
+    <row r="8" spans="2:8" ht="18" thickBot="1">
       <c r="B8" s="7">
         <v>9</v>
       </c>
@@ -3015,68 +5721,68 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:AI21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <cols>
     <col min="2" max="2" width="4.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="4.625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.25" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="4.625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.375" customWidth="1"/>
+    <col min="3" max="3" width="4.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="4.59765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.19921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="4.59765625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.3984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.8984375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.3984375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.3984375" customWidth="1"/>
     <col min="15" max="15" width="4.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.375" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="4.375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.25" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.3984375" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="4.3984375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.19921875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.3984375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="5.875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="4.75" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.3984375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.8984375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="4.69921875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.8984375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:35" ht="17.25" thickBot="1"/>
-    <row r="3" spans="2:35" ht="17.25" thickBot="1">
+    <row r="2" spans="2:35" ht="18" thickBot="1"/>
+    <row r="3" spans="2:35" ht="18" thickBot="1">
       <c r="B3" s="73"/>
       <c r="C3" s="74"/>
-      <c r="D3" s="141" t="s">
+      <c r="D3" s="144" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="146"/>
-      <c r="F3" s="146"/>
-      <c r="G3" s="146"/>
-      <c r="H3" s="146"/>
-      <c r="I3" s="146"/>
-      <c r="J3" s="146"/>
-      <c r="K3" s="146"/>
-      <c r="L3" s="142"/>
-      <c r="M3" s="149" t="s">
+      <c r="E3" s="149"/>
+      <c r="F3" s="149"/>
+      <c r="G3" s="149"/>
+      <c r="H3" s="149"/>
+      <c r="I3" s="149"/>
+      <c r="J3" s="149"/>
+      <c r="K3" s="149"/>
+      <c r="L3" s="145"/>
+      <c r="M3" s="152" t="s">
         <v>81</v>
       </c>
-      <c r="N3" s="149"/>
-      <c r="O3" s="146"/>
-      <c r="P3" s="146"/>
-      <c r="Q3" s="146"/>
-      <c r="R3" s="146"/>
-      <c r="S3" s="146"/>
-      <c r="T3" s="146"/>
-      <c r="U3" s="146"/>
-      <c r="V3" s="146"/>
-      <c r="W3" s="146"/>
-      <c r="X3" s="146"/>
-      <c r="Y3" s="150"/>
+      <c r="N3" s="152"/>
+      <c r="O3" s="149"/>
+      <c r="P3" s="149"/>
+      <c r="Q3" s="149"/>
+      <c r="R3" s="149"/>
+      <c r="S3" s="149"/>
+      <c r="T3" s="149"/>
+      <c r="U3" s="149"/>
+      <c r="V3" s="149"/>
+      <c r="W3" s="149"/>
+      <c r="X3" s="149"/>
+      <c r="Y3" s="153"/>
       <c r="Z3" s="76" t="s">
         <v>57</v>
       </c>
@@ -3085,16 +5791,16 @@
       <c r="B4" s="69"/>
       <c r="C4" s="70"/>
       <c r="D4" s="69"/>
-      <c r="E4" s="145"/>
-      <c r="F4" s="145"/>
-      <c r="G4" s="145"/>
+      <c r="E4" s="148"/>
+      <c r="F4" s="148"/>
+      <c r="G4" s="148"/>
       <c r="H4" s="68"/>
       <c r="I4" s="68"/>
       <c r="J4" s="68"/>
-      <c r="K4" s="143" t="s">
+      <c r="K4" s="146" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="144"/>
+      <c r="L4" s="147"/>
       <c r="M4" s="71"/>
       <c r="N4" s="71"/>
       <c r="O4" s="54"/>
@@ -3104,12 +5810,12 @@
       <c r="S4" s="54"/>
       <c r="T4" s="54"/>
       <c r="U4" s="54"/>
-      <c r="V4" s="147" t="s">
+      <c r="V4" s="150" t="s">
         <v>34</v>
       </c>
-      <c r="W4" s="147"/>
-      <c r="X4" s="147"/>
-      <c r="Y4" s="148"/>
+      <c r="W4" s="150"/>
+      <c r="X4" s="150"/>
+      <c r="Y4" s="151"/>
       <c r="Z4" s="72"/>
       <c r="AC4" t="s">
         <v>101</v>
@@ -3118,7 +5824,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="2:35" ht="17.25" thickBot="1">
+    <row r="5" spans="2:35" ht="18" thickBot="1">
       <c r="B5" s="45"/>
       <c r="C5" s="57" t="s">
         <v>12</v>
@@ -3220,7 +5926,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="2:35" ht="17.25" thickBot="1">
+    <row r="6" spans="2:35" ht="18" thickBot="1">
       <c r="B6" s="12" t="s">
         <v>80</v>
       </c>
@@ -3709,7 +6415,7 @@
       <c r="AA14" s="90"/>
       <c r="AI14" s="93"/>
     </row>
-    <row r="15" spans="2:35" ht="17.25" thickBot="1">
+    <row r="15" spans="2:35" ht="18" thickBot="1">
       <c r="B15" s="7"/>
       <c r="C15" s="60"/>
       <c r="D15" s="7"/>
@@ -3782,21 +6488,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:M13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <sheetData>
     <row r="1" spans="2:13">
       <c r="B1" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="2:13" ht="17.25" thickBot="1">
+    <row r="2" spans="2:13" ht="18" thickBot="1">
       <c r="C2" t="s">
         <v>119</v>
       </c>
@@ -3812,22 +6518,22 @@
         <v>117</v>
       </c>
       <c r="E3" s="114"/>
-      <c r="F3" s="153" t="s">
+      <c r="F3" s="156" t="s">
         <v>106</v>
       </c>
-      <c r="G3" s="153"/>
-      <c r="H3" s="153"/>
-      <c r="I3" s="153" t="s">
+      <c r="G3" s="156"/>
+      <c r="H3" s="156"/>
+      <c r="I3" s="156" t="s">
         <v>96</v>
       </c>
-      <c r="J3" s="153"/>
-      <c r="K3" s="153"/>
-      <c r="L3" s="153"/>
-      <c r="M3" s="151" t="s">
+      <c r="J3" s="156"/>
+      <c r="K3" s="156"/>
+      <c r="L3" s="156"/>
+      <c r="M3" s="154" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="2:13" s="1" customFormat="1" ht="17.25" thickBot="1">
+    <row r="4" spans="2:13" s="1" customFormat="1" ht="18" thickBot="1">
       <c r="B4" s="107" t="s">
         <v>118</v>
       </c>
@@ -3861,7 +6567,7 @@
       <c r="L4" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="M4" s="152"/>
+      <c r="M4" s="155"/>
     </row>
     <row r="5" spans="2:13">
       <c r="B5" s="115">
@@ -3873,7 +6579,7 @@
       <c r="D5" s="54">
         <v>2.04</v>
       </c>
-      <c r="E5" s="156">
+      <c r="E5" s="159">
         <v>3</v>
       </c>
       <c r="F5" s="54">
@@ -3908,7 +6614,7 @@
       <c r="B6" s="4"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="154"/>
+      <c r="E6" s="157"/>
       <c r="F6" s="2">
         <v>32</v>
       </c>
@@ -3941,7 +6647,7 @@
       <c r="B7" s="4"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="154"/>
+      <c r="E7" s="157"/>
       <c r="F7" s="2">
         <v>40</v>
       </c>
@@ -3974,7 +6680,7 @@
       <c r="B8" s="4"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="154"/>
+      <c r="E8" s="157"/>
       <c r="F8" s="2">
         <v>48</v>
       </c>
@@ -4007,7 +6713,7 @@
       <c r="B9" s="4"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="154">
+      <c r="E9" s="157">
         <v>3.5</v>
       </c>
       <c r="F9" s="104">
@@ -4042,7 +6748,7 @@
       <c r="B10" s="4"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="154"/>
+      <c r="E10" s="157"/>
       <c r="F10" s="104">
         <v>32</v>
       </c>
@@ -4075,7 +6781,7 @@
       <c r="B11" s="4"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
-      <c r="E11" s="154">
+      <c r="E11" s="157">
         <v>2.5</v>
       </c>
       <c r="F11" s="2">
@@ -4110,7 +6816,7 @@
       <c r="B12" s="4"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="154"/>
+      <c r="E12" s="157"/>
       <c r="F12" s="2">
         <v>32</v>
       </c>
@@ -4139,11 +6845,11 @@
         <v>23.143750000000004</v>
       </c>
     </row>
-    <row r="13" spans="2:13" ht="17.25" thickBot="1">
+    <row r="13" spans="2:13" ht="18" thickBot="1">
       <c r="B13" s="7"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
-      <c r="E13" s="155"/>
+      <c r="E13" s="158"/>
       <c r="F13" s="110">
         <v>40</v>
       </c>
@@ -4188,84 +6894,84 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B3:AA18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="1" max="1" width="5.125" customWidth="1"/>
-    <col min="2" max="2" width="6.75" customWidth="1"/>
+    <col min="1" max="1" width="5.09765625" customWidth="1"/>
+    <col min="2" max="2" width="6.69921875" customWidth="1"/>
     <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.19921875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.59765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.59765625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="4.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="6.875" customWidth="1"/>
-    <col min="12" max="13" width="6.125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.25" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.25" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="6.8984375" customWidth="1"/>
+    <col min="12" max="13" width="6.09765625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.19921875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.19921875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.09765625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.09765625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="6" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="5.75" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.69921875" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="5.5" customWidth="1"/>
-    <col min="25" max="25" width="7.25" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.75" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="7.19921875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.69921875" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:27" ht="17.25" thickBot="1"/>
+    <row r="3" spans="2:27" ht="18" thickBot="1"/>
     <row r="4" spans="2:27" s="15" customFormat="1">
-      <c r="B4" s="158" t="s">
+      <c r="B4" s="161" t="s">
         <v>126</v>
       </c>
-      <c r="C4" s="153" t="s">
+      <c r="C4" s="156" t="s">
         <v>125</v>
       </c>
-      <c r="D4" s="153"/>
-      <c r="E4" s="153"/>
-      <c r="F4" s="153" t="s">
+      <c r="D4" s="156"/>
+      <c r="E4" s="156"/>
+      <c r="F4" s="156" t="s">
         <v>132</v>
       </c>
-      <c r="G4" s="153"/>
-      <c r="H4" s="153"/>
-      <c r="I4" s="153"/>
-      <c r="J4" s="153"/>
-      <c r="K4" s="153"/>
-      <c r="L4" s="153"/>
-      <c r="M4" s="153" t="s">
+      <c r="G4" s="156"/>
+      <c r="H4" s="156"/>
+      <c r="I4" s="156"/>
+      <c r="J4" s="156"/>
+      <c r="K4" s="156"/>
+      <c r="L4" s="156"/>
+      <c r="M4" s="156" t="s">
         <v>137</v>
       </c>
-      <c r="N4" s="153"/>
-      <c r="O4" s="153"/>
-      <c r="P4" s="153"/>
-      <c r="Q4" s="153"/>
-      <c r="R4" s="153"/>
-      <c r="S4" s="153"/>
-      <c r="T4" s="153"/>
-      <c r="U4" s="160" t="s">
+      <c r="N4" s="156"/>
+      <c r="O4" s="156"/>
+      <c r="P4" s="156"/>
+      <c r="Q4" s="156"/>
+      <c r="R4" s="156"/>
+      <c r="S4" s="156"/>
+      <c r="T4" s="156"/>
+      <c r="U4" s="163" t="s">
         <v>143</v>
       </c>
-      <c r="V4" s="153" t="s">
+      <c r="V4" s="156" t="s">
         <v>144</v>
       </c>
-      <c r="W4" s="153"/>
-      <c r="X4" s="153"/>
-      <c r="Y4" s="153" t="s">
+      <c r="W4" s="156"/>
+      <c r="X4" s="156"/>
+      <c r="Y4" s="156" t="s">
         <v>106</v>
       </c>
-      <c r="Z4" s="153"/>
-      <c r="AA4" s="157"/>
-    </row>
-    <row r="5" spans="2:27" s="15" customFormat="1" ht="17.25" thickBot="1">
-      <c r="B5" s="159"/>
+      <c r="Z4" s="156"/>
+      <c r="AA4" s="160"/>
+    </row>
+    <row r="5" spans="2:27" s="15" customFormat="1" ht="18" thickBot="1">
+      <c r="B5" s="162"/>
       <c r="C5" s="24" t="s">
         <v>127</v>
       </c>
@@ -4318,7 +7024,7 @@
       <c r="T5" s="24" t="s">
         <v>142</v>
       </c>
-      <c r="U5" s="161"/>
+      <c r="U5" s="164"/>
       <c r="V5" s="119" t="s">
         <v>145</v>
       </c>
@@ -4338,7 +7044,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="6" spans="2:27" ht="17.25" thickBot="1">
+    <row r="6" spans="2:27" ht="18" thickBot="1">
       <c r="B6" s="3">
         <v>0.8</v>
       </c>
@@ -4411,7 +7117,7 @@
         <v>21.6</v>
       </c>
     </row>
-    <row r="7" spans="2:27" ht="17.25" thickBot="1">
+    <row r="7" spans="2:27" ht="18" thickBot="1">
       <c r="B7" s="4"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -4467,7 +7173,7 @@
         <v>21.6</v>
       </c>
     </row>
-    <row r="8" spans="2:27" ht="17.25" thickBot="1">
+    <row r="8" spans="2:27" ht="18" thickBot="1">
       <c r="B8" s="7"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
@@ -4699,7 +7405,7 @@
         <v>64.399999999999991</v>
       </c>
     </row>
-    <row r="12" spans="2:27" ht="17.25" thickBot="1">
+    <row r="12" spans="2:27" ht="18" thickBot="1">
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
@@ -5019,7 +7725,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="18" spans="2:27" ht="17.25" thickBot="1">
+    <row r="18" spans="2:27" ht="18" thickBot="1">
       <c r="B18" s="7"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
@@ -5074,16 +7780,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B3:K22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="5" max="5" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:11">
@@ -5283,8 +7989,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="2:11" ht="17.25" thickBot="1"/>
-    <row r="11" spans="2:11" ht="17.25" thickBot="1">
+    <row r="10" spans="2:11" ht="18" thickBot="1"/>
+    <row r="11" spans="2:11" ht="18" thickBot="1">
       <c r="B11" s="131" t="s">
         <v>55</v>
       </c>
@@ -5503,23 +8209,23 @@
       </c>
     </row>
     <row r="19" spans="2:10">
-      <c r="B19" s="162" t="s">
+      <c r="B19" s="165" t="s">
         <v>57</v>
       </c>
-      <c r="C19" s="154" t="s">
+      <c r="C19" s="157" t="s">
         <v>153</v>
       </c>
-      <c r="D19" s="154" t="s">
+      <c r="D19" s="157" t="s">
         <v>154</v>
       </c>
-      <c r="E19" s="154"/>
+      <c r="E19" s="157"/>
       <c r="F19" s="138">
         <v>5</v>
       </c>
       <c r="G19" s="138">
         <v>0.5</v>
       </c>
-      <c r="H19" s="154">
+      <c r="H19" s="157">
         <v>1.6</v>
       </c>
       <c r="I19" s="2">
@@ -5531,17 +8237,17 @@
       </c>
     </row>
     <row r="20" spans="2:10">
-      <c r="B20" s="162"/>
-      <c r="C20" s="154"/>
-      <c r="D20" s="154"/>
-      <c r="E20" s="154"/>
+      <c r="B20" s="165"/>
+      <c r="C20" s="157"/>
+      <c r="D20" s="157"/>
+      <c r="E20" s="157"/>
       <c r="F20" s="138">
         <v>6</v>
       </c>
       <c r="G20" s="138">
         <v>0.6</v>
       </c>
-      <c r="H20" s="154"/>
+      <c r="H20" s="157"/>
       <c r="I20" s="2">
         <v>13.56</v>
       </c>
@@ -5551,32 +8257,32 @@
       </c>
     </row>
     <row r="21" spans="2:10">
-      <c r="B21" s="162"/>
-      <c r="C21" s="154"/>
-      <c r="D21" s="154"/>
-      <c r="E21" s="154"/>
+      <c r="B21" s="165"/>
+      <c r="C21" s="157"/>
+      <c r="D21" s="157"/>
+      <c r="E21" s="157"/>
       <c r="F21" s="138">
         <v>8</v>
       </c>
       <c r="G21" s="138">
         <v>1</v>
       </c>
-      <c r="H21" s="154"/>
+      <c r="H21" s="157"/>
       <c r="I21" s="2"/>
       <c r="J21" s="5"/>
     </row>
-    <row r="22" spans="2:10" ht="17.25" thickBot="1">
-      <c r="B22" s="163"/>
-      <c r="C22" s="155"/>
-      <c r="D22" s="155"/>
-      <c r="E22" s="155"/>
+    <row r="22" spans="2:10" ht="18" thickBot="1">
+      <c r="B22" s="166"/>
+      <c r="C22" s="158"/>
+      <c r="D22" s="158"/>
+      <c r="E22" s="158"/>
       <c r="F22" s="139">
         <v>10</v>
       </c>
       <c r="G22" s="139">
         <v>1.4</v>
       </c>
-      <c r="H22" s="155"/>
+      <c r="H22" s="158"/>
       <c r="I22" s="8"/>
       <c r="J22" s="9"/>
     </row>
@@ -5594,18 +8300,18 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="C4:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="3" max="3" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.09765625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.09765625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="3:11">
@@ -5699,17 +8405,17 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="B4:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <sheetData>
     <row r="4" spans="2:4">
-      <c r="B4" s="164" t="s">
+      <c r="B4" s="167" t="s">
         <v>120</v>
       </c>
       <c r="C4">
@@ -5720,7 +8426,7 @@
       </c>
     </row>
     <row r="5" spans="2:4">
-      <c r="B5" s="164"/>
+      <c r="B5" s="167"/>
       <c r="C5">
         <v>48</v>
       </c>
@@ -5729,7 +8435,7 @@
       </c>
     </row>
     <row r="6" spans="2:4">
-      <c r="B6" s="164"/>
+      <c r="B6" s="167"/>
       <c r="C6">
         <f>C4/C5</f>
         <v>12.5</v>
@@ -5754,79 +8460,79 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="B3:Z18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="1" max="1" width="5.125" customWidth="1"/>
+    <col min="1" max="1" width="5.09765625" customWidth="1"/>
     <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.19921875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.59765625" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="4.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="6.875" customWidth="1"/>
-    <col min="11" max="12" width="6.125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.25" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="6.8984375" customWidth="1"/>
+    <col min="11" max="12" width="6.09765625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.19921875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.19921875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.09765625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.09765625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="6" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.75" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.69921875" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="5.5" customWidth="1"/>
-    <col min="24" max="24" width="7.25" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6.75" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.19921875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.69921875" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:26" ht="17.25" thickBot="1"/>
+    <row r="3" spans="2:26" ht="18" thickBot="1"/>
     <row r="4" spans="2:26" s="15" customFormat="1">
-      <c r="B4" s="153" t="s">
+      <c r="B4" s="156" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="153"/>
-      <c r="D4" s="153"/>
-      <c r="E4" s="153" t="s">
+      <c r="C4" s="156"/>
+      <c r="D4" s="156"/>
+      <c r="E4" s="156" t="s">
         <v>81</v>
       </c>
-      <c r="F4" s="153"/>
-      <c r="G4" s="153"/>
-      <c r="H4" s="153"/>
-      <c r="I4" s="153"/>
-      <c r="J4" s="153"/>
-      <c r="K4" s="153"/>
-      <c r="L4" s="153" t="s">
+      <c r="F4" s="156"/>
+      <c r="G4" s="156"/>
+      <c r="H4" s="156"/>
+      <c r="I4" s="156"/>
+      <c r="J4" s="156"/>
+      <c r="K4" s="156"/>
+      <c r="L4" s="156" t="s">
         <v>57</v>
       </c>
-      <c r="M4" s="153"/>
-      <c r="N4" s="153"/>
-      <c r="O4" s="153"/>
-      <c r="P4" s="153"/>
-      <c r="Q4" s="153"/>
-      <c r="R4" s="153"/>
-      <c r="S4" s="153"/>
-      <c r="T4" s="160" t="s">
+      <c r="M4" s="156"/>
+      <c r="N4" s="156"/>
+      <c r="O4" s="156"/>
+      <c r="P4" s="156"/>
+      <c r="Q4" s="156"/>
+      <c r="R4" s="156"/>
+      <c r="S4" s="156"/>
+      <c r="T4" s="163" t="s">
         <v>100</v>
       </c>
-      <c r="U4" s="153" t="s">
+      <c r="U4" s="156" t="s">
         <v>96</v>
       </c>
-      <c r="V4" s="153"/>
-      <c r="W4" s="153"/>
-      <c r="X4" s="153" t="s">
+      <c r="V4" s="156"/>
+      <c r="W4" s="156"/>
+      <c r="X4" s="156" t="s">
         <v>106</v>
       </c>
-      <c r="Y4" s="153"/>
-      <c r="Z4" s="157"/>
-    </row>
-    <row r="5" spans="2:26" s="15" customFormat="1" ht="17.25" thickBot="1">
+      <c r="Y4" s="156"/>
+      <c r="Z4" s="160"/>
+    </row>
+    <row r="5" spans="2:26" s="15" customFormat="1" ht="18" thickBot="1">
       <c r="B5" s="24" t="s">
         <v>7</v>
       </c>
@@ -5879,7 +8585,7 @@
       <c r="S5" s="24" t="s">
         <v>142</v>
       </c>
-      <c r="T5" s="161"/>
+      <c r="T5" s="164"/>
       <c r="U5" s="119" t="s">
         <v>97</v>
       </c>
@@ -5899,7 +8605,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="6" spans="2:26" ht="17.25" thickBot="1">
+    <row r="6" spans="2:26" ht="18" thickBot="1">
       <c r="B6" s="10">
         <v>0.6</v>
       </c>
@@ -5954,7 +8660,7 @@
         <v>21.6</v>
       </c>
     </row>
-    <row r="7" spans="2:26" ht="17.25" thickBot="1">
+    <row r="7" spans="2:26" ht="18" thickBot="1">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -6003,7 +8709,7 @@
         <v>21.6</v>
       </c>
     </row>
-    <row r="8" spans="2:26" ht="17.25" thickBot="1">
+    <row r="8" spans="2:26" ht="18" thickBot="1">
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
@@ -6191,7 +8897,7 @@
         <v>64.399999999999991</v>
       </c>
     </row>
-    <row r="12" spans="2:26" ht="17.25" thickBot="1">
+    <row r="12" spans="2:26" ht="18" thickBot="1">
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
@@ -6470,7 +9176,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="18" spans="2:26" ht="17.25" thickBot="1">
+    <row r="18" spans="2:26" ht="18" thickBot="1">
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>

</xml_diff>